<commit_message>
Updated survey results (#10)
* Added culminating readme
* Added more information to culminating readme
* Added link to Google Form
* Added survey results
* Re-added survey responses
* Fixed some whiteline inconsistencies
* Updated survey results
* Updated survey results
</commit_message>
<xml_diff>
--- a/Assignments/10 - Culminating/Survey_Responses.xlsx
+++ b/Assignments/10 - Culminating/Survey_Responses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Dropbox\My Documents\Queens\Practica\PRAC 461\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Documents\GitHub\ICS3C\Assignments\10 - Culminating\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
   <si>
     <t>What is your name?</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Knowing the news</t>
   </si>
   <si>
-    <t>Programming</t>
-  </si>
-  <si>
     <t>So you know what to do when your computer is broken</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Not cyberbullying</t>
   </si>
   <si>
-    <t>Film editing</t>
-  </si>
-  <si>
     <t>It allows us to stay in touch with the advancing times as we know them</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t xml:space="preserve">Video Game designer </t>
   </si>
   <si>
-    <t xml:space="preserve">It's helpful for the future of technology </t>
-  </si>
-  <si>
     <t>Arva</t>
   </si>
   <si>
@@ -180,9 +171,6 @@
     <t>Digital Communication</t>
   </si>
   <si>
-    <t>Helps one develop better problem solving skills</t>
-  </si>
-  <si>
     <t>Jenny</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t>Being honest</t>
   </si>
   <si>
-    <t>Computer engineering</t>
-  </si>
-  <si>
     <t>Bhavya</t>
   </si>
   <si>
@@ -271,6 +256,24 @@
   </si>
   <si>
     <t>Not being a jerk</t>
+  </si>
+  <si>
+    <t>Miss Strong</t>
+  </si>
+  <si>
+    <t>Not trolling</t>
+  </si>
+  <si>
+    <t>Film editor</t>
+  </si>
+  <si>
+    <t>You learn how to think critically and systematically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is helpful for the future of technology </t>
+  </si>
+  <si>
+    <t>Helps you develop better problem solving skills</t>
   </si>
 </sst>
 </file>
@@ -625,11 +628,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -663,267 +666,267 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>50</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1">
-        <v>80</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1">
         <v>8</v>
       </c>
       <c r="C14" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -932,98 +935,98 @@
         <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B16" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1">
+        <v>80</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1">
-        <v>70</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1">
         <v>7</v>
@@ -1032,56 +1035,79 @@
         <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1">
+        <v>70</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>80</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="1">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>80</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>82</v>
+      <c r="F23" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F23">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>